<commit_message>
add mapping prompt model
</commit_message>
<xml_diff>
--- a/dbms-mvc.Tests/Files/test-spreadsheet-invalid-col-names.xlsx
+++ b/dbms-mvc.Tests/Files/test-spreadsheet-invalid-col-names.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">Organization</t>
   </si>
   <si>
-    <t xml:space="preserve">FirstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LastName</t>
+    <t xml:space="preserve">The First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Last Name</t>
   </si>
   <si>
     <t xml:space="preserve">Combined Name</t>
@@ -37,10 +37,10 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">StreetAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StreetAddress2</t>
+    <t xml:space="preserve">Address Of Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary Company Address</t>
   </si>
   <si>
     <t xml:space="preserve">City</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Province</t>
   </si>
   <si>
-    <t xml:space="preserve">Postal Code</t>
+    <t xml:space="preserve">Postal</t>
   </si>
   <si>
     <t xml:space="preserve">Phone</t>
@@ -61,16 +61,16 @@
     <t xml:space="preserve">Website</t>
   </si>
   <si>
-    <t xml:space="preserve">HomeCategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MailingList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BedsCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subscribed</t>
+    <t xml:space="preserve">Category Of Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which Mailing List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of beds ###</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subscribed?</t>
   </si>
   <si>
     <t xml:space="preserve">Emails</t>
@@ -260,28 +260,32 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,230 +369,230 @@
   </sheetPr>
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P10" activeCellId="0" sqref="P10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="2" t="str">
+      <c r="D2" s="3" t="str">
         <f aca="false">B2&amp;" "&amp;C2</f>
         <v>Roslyn Schultz</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="P2" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="str">
+      <c r="D3" s="3" t="str">
         <f aca="false">B3&amp;" "&amp;C3</f>
         <v>Eric Chartrand</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="2" t="n">
+      <c r="P3" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="2" t="str">
+      <c r="D4" s="3" t="str">
         <f aca="false">B4&amp;" "&amp;C4</f>
         <v>Sahra Nilayeh</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="5"/>
+      <c r="H4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4" t="s">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>